<commit_message>
Updated so that CSV export actually worksUpdated so that export to CSV actually works
</commit_message>
<xml_diff>
--- a/Test Data.xlsx
+++ b/Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w.saunders\source\repos\AlumniEngagementScore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EA2653E-F604-42E5-8EEF-CB16730F2507}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7B0F1C-6313-4997-8801-6671430E4A83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{19B6DE30-6F43-4D18-B535-ED47231F4420}"/>
+    <workbookView xWindow="-14625" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{19B6DE30-6F43-4D18-B535-ED47231F4420}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>Bill</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>Sally</t>
   </si>
 </sst>
 </file>
@@ -412,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED251AD4-E9DF-4660-A85B-1DA635E242FF}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,46 +454,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>164379</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>21</v>
-      </c>
-      <c r="D3">
-        <v>145</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>59</v>
-      </c>
-      <c r="D4">
-        <v>51</v>
-      </c>
-      <c r="E4">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>